<commit_message>
Fix Enum val is empty
</commit_message>
<xml_diff>
--- a/Demo/Data/0_no_loc/data/Item2.xlsx
+++ b/Demo/Data/0_no_loc/data/Item2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fancyHub\ExportExcel\TestData\0_no_loc\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fancyHub\ExportExcel\Demo\Data\0_no_loc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD2CBDB-45EE-4C06-B7C3-8376083E1631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9629226B-3E9A-43FE-A6A7-CAA18081E466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>#remark</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -52,10 +52,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>类型</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>灰色</t>
   </si>
   <si>
@@ -64,9 +60,6 @@
   <si>
     <t>品质</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>武器</t>
   </si>
   <si>
     <t>手枪</t>
@@ -81,11 +74,6 @@
   </si>
   <si>
     <t>int
-Enum[EItemType]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>int
 Enum[EItemSubType]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -101,10 +89,6 @@
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -548,10 +532,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -559,51 +543,44 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="23.25" customWidth="1"/>
     <col min="3" max="3" width="9.625" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.75" customWidth="1"/>
+    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -614,47 +591,38 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -664,22 +632,22 @@
       <formula>公式单元格=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:F1048576 G2">
+  <conditionalFormatting sqref="D1:E1048576 F2">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="紫色">
-      <formula>NOT(ISERROR(SEARCH("紫色",E1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("紫色",D1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="灰色">
-      <formula>NOT(ISERROR(SEARCH("灰色",E1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("灰色",D1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="绿色">
-      <formula>NOT(ISERROR(SEARCH("绿色",E1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("绿色",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:F5" xr:uid="{E0340732-8881-4BC9-A7C2-7D237ABA5FF0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E5" xr:uid="{E0340732-8881-4BC9-A7C2-7D237ABA5FF0}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D5 F4:F5" xr:uid="{ABA0D88B-5028-40B8-BC94-1B76F6C1355E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E5" xr:uid="{ABA0D88B-5028-40B8-BC94-1B76F6C1355E}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>